<commit_message>
doc: add project report and team worklog documents
</commit_message>
<xml_diff>
--- a/docs/worklogs/Bryan_Zweiacker_worklog.xlsx
+++ b/docs/worklogs/Bryan_Zweiacker_worklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sytabram/Documents/SynologyDrive/CPNV/MA-Métier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049BD32D-469E-A649-863B-CC4A2F642FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BED35A-FEAA-D94C-9D75-B36D32E1B095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63040" yWindow="6340" windowWidth="26320" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="660" windowWidth="26320" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
   <si>
     <t>Jour</t>
   </si>
@@ -148,6 +148,27 @@
   <si>
     <t>Problèmes de connexion à la manette à cause de l'adresse MAC</t>
   </si>
+  <si>
+    <t>mercredi, 21 janvier 2026</t>
+  </si>
+  <si>
+    <t>Sécurisation du github avec des branch rules et CodeOwners</t>
+  </si>
+  <si>
+    <t>Suite à un problème sur la branche main, il a été décidé d'ajouter des règles sur le répo. // Problème: J'ai dû apprendre à faire des rules</t>
+  </si>
+  <si>
+    <t>jeudi, 22 janvier 2026</t>
+  </si>
+  <si>
+    <t>Liaison contrôleur PS4 avec le moteur de direction</t>
+  </si>
+  <si>
+    <t>Test sur la voiture du système de direction et correction de l'axe</t>
+  </si>
+  <si>
+    <t>Merge de la branche Steper-Mottor, répartition du code dans un class distincte</t>
+  </si>
 </sst>
 </file>
 
@@ -156,9 +177,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
@@ -219,12 +247,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -236,38 +264,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -280,9 +317,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,16 +937,16 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.75</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1934,7 +1968,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2218,7 +2252,7 @@
       <c r="D15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="23" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="8"/>
@@ -2242,51 +2276,113 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="14">
+        <v>2</v>
+      </c>
+      <c r="C17" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="A18" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="14">
+        <v>2</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="6"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="14">
+        <v>2</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1.75</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>42</v>
+      </c>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="14">
+        <v>2</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="14">
+        <v>2</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="6"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="14">
+        <v>2</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6114,7 +6210,7 @@
       <c r="F500" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B300" xr:uid="{E1FCDE41-ACF1-4A68-9483-C062BB428146}">
       <formula1>1</formula1>
@@ -6195,7 +6291,7 @@
       </c>
       <c r="B4" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>9</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6204,7 +6300,7 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6213,7 +6309,7 @@
       </c>
       <c r="B6" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>1.25</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6222,7 +6318,7 @@
       </c>
       <c r="B7" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>2.75</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
doc: update worklogs for Bryan, Ilyass, and Trystan
</commit_message>
<xml_diff>
--- a/docs/worklogs/Bryan_Zweiacker_worklog.xlsx
+++ b/docs/worklogs/Bryan_Zweiacker_worklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sytabram/Documents/SynologyDrive/CPNV/MA-Métier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BED35A-FEAA-D94C-9D75-B36D32E1B095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4408902-B3CA-8242-A6F1-F1B6EB8E601B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="660" windowWidth="26320" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="660" windowWidth="30100" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
   <si>
     <t>Jour</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Réception complète des données bluetooth de la manette</t>
   </si>
   <si>
-    <t xml:space="preserve">Structure et architecture du code </t>
-  </si>
-  <si>
     <t>Séance avec les membres du projet</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>Review code avant merge</t>
   </si>
   <si>
-    <t>Refactoring code en classes distinctes</t>
-  </si>
-  <si>
     <t>Liaison contrôleur PS4 avec LED</t>
   </si>
   <si>
@@ -150,12 +144,6 @@
   </si>
   <si>
     <t>mercredi, 21 janvier 2026</t>
-  </si>
-  <si>
-    <t>Sécurisation du github avec des branch rules et CodeOwners</t>
-  </si>
-  <si>
-    <t>Suite à un problème sur la branche main, il a été décidé d'ajouter des règles sur le répo. // Problème: J'ai dû apprendre à faire des rules</t>
   </si>
   <si>
     <t>jeudi, 22 janvier 2026</t>
@@ -167,7 +155,49 @@
     <t>Test sur la voiture du système de direction et correction de l'axe</t>
   </si>
   <si>
-    <t>Merge de la branche Steper-Mottor, répartition du code dans un class distincte</t>
+    <t>vendredi, 23 janvier 2026</t>
+  </si>
+  <si>
+    <t>Merge de la branche led-braking sur develop et refactorisation</t>
+  </si>
+  <si>
+    <t>lundi, 26 janvier 2026</t>
+  </si>
+  <si>
+    <t>mardi, 27 janvier 2026</t>
+  </si>
+  <si>
+    <t>Refactoring code complet pour séparer en classes distinctes</t>
+  </si>
+  <si>
+    <t>Prise en charge des phares RGB au démarrage</t>
+  </si>
+  <si>
+    <t>Mise à jour du journal de travail</t>
+  </si>
+  <si>
+    <t>Structure et architecture du code</t>
+  </si>
+  <si>
+    <t>Sécurisation du GitHub avec des branch rules et CodeOwners</t>
+  </si>
+  <si>
+    <t>Suite à un problème sur la branche main, ajout de règles sur le répo. Apprentissage nécessaire pour configurer les rules</t>
+  </si>
+  <si>
+    <t>Merge de la branche Stepper-Motor, répartition du code dans une classe distincte</t>
+  </si>
+  <si>
+    <t>Test de la feature led-braking</t>
+  </si>
+  <si>
+    <t>Correction des pins de freins et fermeture de la pull request</t>
+  </si>
+  <si>
+    <t>Merge et refactorisation de la branche warning</t>
+  </si>
+  <si>
+    <t>Test de toutes les fonctionnalités liées aux LED et corrections</t>
   </si>
 </sst>
 </file>
@@ -177,9 +207,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
@@ -247,12 +284,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -264,38 +301,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -308,9 +354,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -937,16 +980,16 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.25</c:v>
+                  <c:v>22.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.75</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1968,7 +2011,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2003,7 +2046,7 @@
     </row>
     <row r="2" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="14">
         <v>1</v>
@@ -2021,7 +2064,7 @@
     </row>
     <row r="3" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="14">
         <v>1</v>
@@ -2039,7 +2082,7 @@
     </row>
     <row r="4" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="14">
         <v>1</v>
@@ -2051,13 +2094,13 @@
         <v>7</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="14">
         <v>1</v>
@@ -2069,13 +2112,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="14">
         <v>1</v>
@@ -2095,7 +2138,7 @@
     </row>
     <row r="7" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="14">
         <v>1</v>
@@ -2110,12 +2153,12 @@
         <v>19</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="14">
         <v>1</v>
@@ -2127,13 +2170,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="14">
         <v>1</v>
@@ -2151,7 +2194,7 @@
     </row>
     <row r="10" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="14">
         <v>1</v>
@@ -2163,13 +2206,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="14">
         <v>1</v>
@@ -2181,13 +2224,13 @@
         <v>6</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="14">
         <v>1</v>
@@ -2199,13 +2242,13 @@
         <v>9</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="14">
         <v>2</v>
@@ -2216,14 +2259,14 @@
       <c r="D13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>27</v>
+      <c r="E13" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="14">
         <v>2</v>
@@ -2234,14 +2277,14 @@
       <c r="D14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>33</v>
+      <c r="E14" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="14">
         <v>2</v>
@@ -2253,13 +2296,13 @@
         <v>9</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="14">
         <v>2</v>
@@ -2271,13 +2314,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="14">
         <v>2</v>
@@ -2289,13 +2332,13 @@
         <v>9</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="14">
         <v>2</v>
@@ -2307,15 +2350,15 @@
         <v>6</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B19" s="14">
         <v>2</v>
@@ -2327,13 +2370,13 @@
         <v>9</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" s="14">
         <v>2</v>
@@ -2345,13 +2388,13 @@
         <v>9</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B21" s="14">
         <v>2</v>
@@ -2363,13 +2406,13 @@
         <v>10</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B22" s="14">
         <v>2</v>
@@ -2381,72 +2424,152 @@
         <v>11</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2</v>
+      </c>
+      <c r="C23" s="11">
+        <v>2.75</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>39</v>
+      </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="6"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="14">
+        <v>2</v>
+      </c>
+      <c r="C24" s="11">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>20</v>
+      </c>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="6"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="14">
+        <v>3</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>49</v>
+      </c>
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="6"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="8"/>
+      <c r="A26" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="14">
+        <v>3</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>50</v>
+      </c>
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="14">
+        <v>3</v>
+      </c>
+      <c r="C27" s="11">
+        <v>2</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>51</v>
+      </c>
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="6"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="14">
+        <v>3</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="14">
+        <v>3</v>
+      </c>
+      <c r="C29" s="11">
+        <v>1.75</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>43</v>
+      </c>
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="6"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="14">
+        <v>3</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>44</v>
+      </c>
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6210,7 +6333,7 @@
       <c r="F500" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B300" xr:uid="{E1FCDE41-ACF1-4A68-9483-C062BB428146}">
       <formula1>1</formula1>
@@ -6223,9 +6346,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B1:D1" listDataValidation="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -6291,7 +6411,7 @@
       </c>
       <c r="B4" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>15.25</v>
+        <v>22.25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6300,7 +6420,7 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6318,7 +6438,7 @@
       </c>
       <c r="B7" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>4.75</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
doc: update project report and worklog documents
</commit_message>
<xml_diff>
--- a/docs/worklogs/Bryan_Zweiacker_worklog.xlsx
+++ b/docs/worklogs/Bryan_Zweiacker_worklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10125"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sytabram/Documents/SynologyDrive/CPNV/MA-Métier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4408902-B3CA-8242-A6F1-F1B6EB8E601B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7852C9F2-19C8-9348-B7B2-580C9B0B8030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="660" windowWidth="30100" windowHeight="21680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="62">
   <si>
     <t>Jour</t>
   </si>
@@ -199,6 +199,33 @@
   <si>
     <t>Test de toutes les fonctionnalités liées aux LED et corrections</t>
   </si>
+  <si>
+    <t>mercredi, 28 janvier 2026</t>
+  </si>
+  <si>
+    <t>Merge et refactorisation de la branche capteur-ultra-son</t>
+  </si>
+  <si>
+    <t>Ajout de la logique moteur et création du mode "auto"</t>
+  </si>
+  <si>
+    <t>jeudi, 29 janvier 2026</t>
+  </si>
+  <si>
+    <t>Test moteur, freinage d'urgence et mode auto</t>
+  </si>
+  <si>
+    <t>La feature a dû être faite sans pouvoir tester car le moteur n'était pas encore prêt</t>
+  </si>
+  <si>
+    <t>PowerPoint pour le pitch</t>
+  </si>
+  <si>
+    <t>Problèmes avec le loop du capteur ultrason qui bloque toutes les autres fonctionnalités, correction de divers bugs liés au moteur</t>
+  </si>
+  <si>
+    <t>Portes ouvertes</t>
+  </si>
 </sst>
 </file>
 
@@ -207,9 +234,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
@@ -284,12 +318,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -301,38 +335,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -346,9 +389,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -357,6 +397,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -980,13 +1023,13 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.25</c:v>
+                  <c:v>26.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.75</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.75</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.25</c:v>
@@ -995,7 +1038,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2010,8 +2053,8 @@
   <dimension ref="A1:F500"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2513,7 +2556,7 @@
       <c r="D27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="28" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="8"/>
@@ -2573,43 +2616,97 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="6"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
+      <c r="A31" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="14">
+        <v>3</v>
+      </c>
+      <c r="C31" s="11">
+        <v>2</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="6"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="A32" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14">
+        <v>3</v>
+      </c>
+      <c r="C32" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="6"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="8"/>
+      <c r="A33" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="14">
+        <v>3</v>
+      </c>
+      <c r="C33" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>59</v>
+      </c>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="6"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="A34" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="14">
+        <v>3</v>
+      </c>
+      <c r="C34" s="11">
+        <v>3</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="6"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
+      <c r="A35" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="14">
+        <v>3</v>
+      </c>
+      <c r="C35" s="11">
+        <v>1.25</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6333,7 +6430,7 @@
       <c r="F500" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B300" xr:uid="{E1FCDE41-ACF1-4A68-9483-C062BB428146}">
       <formula1>1</formula1>
@@ -6411,7 +6508,7 @@
       </c>
       <c r="B4" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>22.25</v>
+        <v>26.75</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6420,7 +6517,7 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>2.75</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6429,7 +6526,7 @@
       </c>
       <c r="B6" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>2.75</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -6456,7 +6553,7 @@
       </c>
       <c r="B9" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>